<commit_message>
removing old files and updating templates
</commit_message>
<xml_diff>
--- a/projects/training_lhs1.xlsx
+++ b/projects/training_lhs1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19840" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27640" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -4061,10 +4061,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1481">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5848,8 +5848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5977,7 +5977,7 @@
         <v>460</v>
       </c>
       <c r="B9" s="27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="36" t="s">
@@ -5985,7 +5985,7 @@
       </c>
       <c r="E9" s="36" t="str">
         <f>"$"&amp;VALUE(LEFT(E7,5))+B9*VALUE(LEFT(E8,5))&amp;"/hour"</f>
-        <v>$3.85/hour</v>
+        <v>$2.17/hour</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>609</v>
@@ -6097,7 +6097,7 @@
         <v>453</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>554</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="33" customFormat="1">
@@ -6126,7 +6126,7 @@
     <row r="24" spans="1:6">
       <c r="A24" s="33" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,1,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,1,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))</f>
-        <v>popSize</v>
+        <v>Sample Method</v>
       </c>
       <c r="B24" s="28" t="str">
         <f>IF(D24&lt;&gt;"",D24,IF(LEN(INDEX(Lookups!$C$21:$Z$30,1,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,1,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1)))</f>
@@ -6134,7 +6134,7 @@
       </c>
       <c r="C24" s="37" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,1,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,1,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))</f>
-        <v>Size of initial population</v>
+        <v>individual_variables / all_variables</v>
       </c>
       <c r="D24" s="39" t="s">
         <v>454</v>
@@ -6144,7 +6144,7 @@
     <row r="25" spans="1:6">
       <c r="A25" s="33" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))</f>
-        <v>Generations</v>
+        <v>Number of Samples</v>
       </c>
       <c r="B25" s="28">
         <f>IF(D25&lt;&gt;"",D25,IF(LEN(INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1)))</f>
@@ -6152,7 +6152,7 @@
       </c>
       <c r="C25" s="37" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,2,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))</f>
-        <v>Number of generations</v>
+        <v>positive integer (if individual, total simulations is this times each variable)</v>
       </c>
       <c r="D25" s="39">
         <v>300</v>
@@ -6162,15 +6162,15 @@
     <row r="26" spans="1:6" ht="28">
       <c r="A26" s="33" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,3,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,3,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))</f>
-        <v>waitGenerations</v>
-      </c>
-      <c r="B26" s="28">
+        <v/>
+      </c>
+      <c r="B26" s="28" t="str">
         <f>IF(D26&lt;&gt;"",D26,IF(LEN(INDEX(Lookups!$C$21:$Z$30,3,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,3,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1)))</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="C26" s="37" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,3,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,3,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))</f>
-        <v>If no improvement in waitGenerations of generations, then exit</v>
+        <v/>
       </c>
       <c r="D26" s="39"/>
       <c r="E26" s="33"/>
@@ -6178,101 +6178,101 @@
     <row r="27" spans="1:6" s="33" customFormat="1" ht="28">
       <c r="A27" s="33" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,4,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,4,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))</f>
-        <v>bfgsburnin</v>
-      </c>
-      <c r="B27" s="28">
+        <v/>
+      </c>
+      <c r="B27" s="28" t="str">
         <f>IF(D27&lt;&gt;"",D27,IF(LEN(INDEX(Lookups!$C$21:$Z$30,4,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,4,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1)))</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="C27" s="37" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,4,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,4,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))</f>
-        <v>The number of generations which are run before the BFGS is ﬁrst used</v>
+        <v/>
       </c>
       <c r="D27" s="39"/>
     </row>
     <row r="28" spans="1:6" s="33" customFormat="1" ht="28">
       <c r="A28" s="33" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,5,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,5,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))</f>
-        <v>solutionTolerance</v>
-      </c>
-      <c r="B28" s="28">
+        <v/>
+      </c>
+      <c r="B28" s="28" t="str">
         <f>IF(D28&lt;&gt;"",D28,IF(LEN(INDEX(Lookups!$C$21:$Z$30,5,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,5,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1)))</f>
-        <v>0.01</v>
+        <v/>
       </c>
       <c r="C28" s="37" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,5,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,5,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))</f>
-        <v>Numbers within solutionTolerance are considered equal</v>
+        <v/>
       </c>
       <c r="D28" s="39"/>
     </row>
     <row r="29" spans="1:6" s="33" customFormat="1">
       <c r="A29" s="33" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,6,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,6,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))</f>
-        <v>epsilonGradient</v>
-      </c>
-      <c r="B29" s="28">
+        <v/>
+      </c>
+      <c r="B29" s="28" t="str">
         <f>IF(D29&lt;&gt;"",D29,IF(LEN(INDEX(Lookups!$C$21:$Z$30,6,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,6,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1)))</f>
-        <v>0.01</v>
+        <v/>
       </c>
       <c r="C29" s="37" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,6,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,6,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))</f>
-        <v>epsilon in gradient calculation</v>
+        <v/>
       </c>
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:6" s="33" customFormat="1">
       <c r="A30" s="33" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,7,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,7,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))</f>
-        <v>pgtol</v>
-      </c>
-      <c r="B30" s="28">
+        <v/>
+      </c>
+      <c r="B30" s="28" t="str">
         <f>IF(D30&lt;&gt;"",D30,IF(LEN(INDEX(Lookups!$C$21:$Z$30,7,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,7,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1)))</f>
-        <v>0.01</v>
+        <v/>
       </c>
       <c r="C30" s="37" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,7,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,7,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))</f>
-        <v>tolerance on the projected gradient</v>
+        <v/>
       </c>
       <c r="D30" s="39"/>
     </row>
     <row r="31" spans="1:6" s="33" customFormat="1">
       <c r="A31" s="33" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,8,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,8,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))</f>
-        <v>factr</v>
-      </c>
-      <c r="B31" s="28">
+        <v/>
+      </c>
+      <c r="B31" s="28" t="str">
         <f>IF(D31&lt;&gt;"",D31,IF(LEN(INDEX(Lookups!$C$21:$Z$30,8,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,8,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1)))</f>
-        <v>45036000000000</v>
+        <v/>
       </c>
       <c r="C31" s="37" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,8,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,8,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))</f>
-        <v>Tolerance on delta_F</v>
+        <v/>
       </c>
       <c r="D31" s="39"/>
     </row>
     <row r="32" spans="1:6" s="33" customFormat="1">
       <c r="A32" s="33" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,9,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,9,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))</f>
-        <v>maxit</v>
-      </c>
-      <c r="B32" s="28">
+        <v/>
+      </c>
+      <c r="B32" s="28" t="str">
         <f>IF(D32&lt;&gt;"",D32,IF(LEN(INDEX(Lookups!$C$21:$Z$30,9,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,9,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1)))</f>
-        <v>100</v>
+        <v/>
       </c>
       <c r="C32" s="37" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,9,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,9,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))</f>
-        <v>Maximum number of iterations</v>
+        <v/>
       </c>
       <c r="D32" s="39"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="33" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,10,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$30,10,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))</f>
-        <v>normType</v>
+        <v/>
       </c>
       <c r="B33" s="28" t="str">
         <f>IF(D33&lt;&gt;"",D33,IF(LEN(INDEX(Lookups!$C$21:$Z$30,10,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$30,10,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1)))</f>
-        <v>minkowski</v>
+        <v/>
       </c>
       <c r="C33" s="37" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$30,10,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$30,10,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))</f>
@@ -6284,15 +6284,15 @@
     <row r="34" spans="1:6" s="33" customFormat="1">
       <c r="A34" s="33" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$31,11,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))=0,"",INDEX(Lookups!$C$21:$Z$31,11,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-2))</f>
-        <v>pPower</v>
-      </c>
-      <c r="B34" s="28">
+        <v/>
+      </c>
+      <c r="B34" s="28" t="str">
         <f>IF(D34&lt;&gt;"",D34,IF(LEN(INDEX(Lookups!$C$21:$Z$31,11,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1))=0,"",INDEX(Lookups!$C$21:$Z$31,11,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)-1)))</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="C34" s="37" t="str">
         <f>IF(LEN(INDEX(Lookups!$C$21:$Z$31,11,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))=0,"",INDEX(Lookups!$C$21:$Z$31,11,3*MATCH(Setup!$B21,Lookups!$A$21:$A$27,0)))</f>
-        <v>Lp norm power</v>
+        <v/>
       </c>
       <c r="D34" s="39"/>
     </row>
@@ -6408,7 +6408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -6465,14 +6465,14 @@
       <c r="R1" s="24"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
-      <c r="U1" s="43" t="s">
+      <c r="U1" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
-      <c r="X1" s="43"/>
-      <c r="Y1" s="43"/>
-      <c r="Z1" s="43"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
     </row>
     <row r="2" spans="1:26" s="8" customFormat="1" ht="15">
       <c r="A2" s="8" t="s">
@@ -6567,20 +6567,20 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="44" customFormat="1">
-      <c r="A4" s="44" t="b">
+    <row r="4" spans="1:26" s="43" customFormat="1">
+      <c r="A4" s="43" t="b">
         <v>1</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="43" t="s">
         <v>680</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="43" t="s">
         <v>681</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="43" t="s">
         <v>681</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="43" t="s">
         <v>68</v>
       </c>
     </row>
@@ -6741,20 +6741,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:26" s="44" customFormat="1">
-      <c r="A12" s="44" t="b">
+    <row r="12" spans="1:26" s="43" customFormat="1">
+      <c r="A12" s="43" t="b">
         <v>1</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="43" t="s">
         <v>383</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="43" t="s">
         <v>684</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="44" t="s">
+      <c r="E12" s="43" t="s">
         <v>68</v>
       </c>
     </row>
@@ -6828,20 +6828,20 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:26" s="44" customFormat="1">
-      <c r="A16" s="44" t="b">
+    <row r="16" spans="1:26" s="43" customFormat="1">
+      <c r="A16" s="43" t="b">
         <v>1</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="43" t="s">
         <v>383</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="43" t="s">
         <v>684</v>
       </c>
-      <c r="D16" s="44" t="s">
+      <c r="D16" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="E16" s="44" t="s">
+      <c r="E16" s="43" t="s">
         <v>68</v>
       </c>
     </row>
@@ -6915,20 +6915,20 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:18" s="44" customFormat="1">
-      <c r="A20" s="44" t="b">
+    <row r="20" spans="1:18" s="43" customFormat="1">
+      <c r="A20" s="43" t="b">
         <v>1</v>
       </c>
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="43" t="s">
         <v>383</v>
       </c>
-      <c r="C20" s="44" t="s">
+      <c r="C20" s="43" t="s">
         <v>684</v>
       </c>
-      <c r="D20" s="44" t="s">
+      <c r="D20" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="E20" s="44" t="s">
+      <c r="E20" s="43" t="s">
         <v>68</v>
       </c>
     </row>
@@ -6986,20 +6986,20 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:18" s="44" customFormat="1">
-      <c r="A24" s="44" t="b">
+    <row r="24" spans="1:18" s="43" customFormat="1">
+      <c r="A24" s="43" t="b">
         <v>1</v>
       </c>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="43" t="s">
         <v>383</v>
       </c>
-      <c r="C24" s="44" t="s">
+      <c r="C24" s="43" t="s">
         <v>684</v>
       </c>
-      <c r="D24" s="44" t="s">
+      <c r="D24" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="E24" s="44" t="s">
+      <c r="E24" s="43" t="s">
         <v>68</v>
       </c>
     </row>
@@ -7057,20 +7057,20 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:18" s="44" customFormat="1">
-      <c r="A28" s="44" t="b">
+    <row r="28" spans="1:18" s="43" customFormat="1">
+      <c r="A28" s="43" t="b">
         <v>1</v>
       </c>
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="43" t="s">
         <v>687</v>
       </c>
-      <c r="C28" s="44" t="s">
+      <c r="C28" s="43" t="s">
         <v>688</v>
       </c>
-      <c r="D28" s="44" t="s">
+      <c r="D28" s="43" t="s">
         <v>689</v>
       </c>
-      <c r="E28" s="44" t="s">
+      <c r="E28" s="43" t="s">
         <v>68</v>
       </c>
     </row>
@@ -7151,20 +7151,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:18" s="44" customFormat="1">
-      <c r="A33" s="44" t="b">
+    <row r="33" spans="1:18" s="43" customFormat="1">
+      <c r="A33" s="43" t="b">
         <v>1</v>
       </c>
-      <c r="B33" s="44" t="s">
+      <c r="B33" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="C33" s="44" t="s">
+      <c r="C33" s="43" t="s">
         <v>702</v>
       </c>
-      <c r="D33" s="44" t="s">
+      <c r="D33" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="E33" s="44" t="s">
+      <c r="E33" s="43" t="s">
         <v>68</v>
       </c>
     </row>
@@ -7258,20 +7258,20 @@
         <v>704</v>
       </c>
     </row>
-    <row r="38" spans="1:18" s="44" customFormat="1">
-      <c r="A38" s="44" t="b">
+    <row r="38" spans="1:18" s="43" customFormat="1">
+      <c r="A38" s="43" t="b">
         <v>1</v>
       </c>
-      <c r="B38" s="44" t="s">
+      <c r="B38" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="C38" s="44" t="s">
+      <c r="C38" s="43" t="s">
         <v>702</v>
       </c>
-      <c r="D38" s="44" t="s">
+      <c r="D38" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="E38" s="44" t="s">
+      <c r="E38" s="43" t="s">
         <v>68</v>
       </c>
     </row>
@@ -7365,20 +7365,20 @@
         <v>704</v>
       </c>
     </row>
-    <row r="43" spans="1:18" s="44" customFormat="1">
-      <c r="A43" s="44" t="b">
+    <row r="43" spans="1:18" s="43" customFormat="1">
+      <c r="A43" s="43" t="b">
         <v>1</v>
       </c>
-      <c r="B43" s="44" t="s">
+      <c r="B43" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="C43" s="44" t="s">
+      <c r="C43" s="43" t="s">
         <v>702</v>
       </c>
-      <c r="D43" s="44" t="s">
+      <c r="D43" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="E43" s="44" t="s">
+      <c r="E43" s="43" t="s">
         <v>68</v>
       </c>
     </row>
@@ -7472,20 +7472,20 @@
         <v>704</v>
       </c>
     </row>
-    <row r="48" spans="1:18" s="44" customFormat="1">
-      <c r="A48" s="44" t="b">
+    <row r="48" spans="1:18" s="43" customFormat="1">
+      <c r="A48" s="43" t="b">
         <v>1</v>
       </c>
-      <c r="B48" s="44" t="s">
+      <c r="B48" s="43" t="s">
         <v>707</v>
       </c>
-      <c r="C48" s="44" t="s">
+      <c r="C48" s="43" t="s">
         <v>708</v>
       </c>
-      <c r="D48" s="44" t="s">
+      <c r="D48" s="43" t="s">
         <v>709</v>
       </c>
-      <c r="E48" s="44" t="s">
+      <c r="E48" s="43" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>

<commit_message>
training measures, sudo notes, and clean logs
</commit_message>
<xml_diff>
--- a/projects/training_lhs1.xlsx
+++ b/projects/training_lhs1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="562"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19840" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2292,9 +2292,6 @@
     <t>$</t>
   </si>
   <si>
-    <t>../TrainingMeasures</t>
-  </si>
-  <si>
     <t>East PF</t>
   </si>
   <si>
@@ -2347,6 +2344,9 @@
   </si>
   <si>
     <t>0.3.5</t>
+  </si>
+  <si>
+    <t>../training_measures</t>
   </si>
 </sst>
 </file>
@@ -4062,11 +4062,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1481">
@@ -5852,7 +5852,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5889,8 +5889,8 @@
       <c r="A3" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="B3" s="45" t="s">
-        <v>768</v>
+      <c r="B3" s="44" t="s">
+        <v>767</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>437</v>
@@ -5912,7 +5912,7 @@
         <v>471</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>618</v>
@@ -6020,7 +6020,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>750</v>
+        <v>768</v>
       </c>
       <c r="F13" s="33" t="s">
         <v>619</v>
@@ -6468,14 +6468,14 @@
       <c r="R1" s="24"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
-      <c r="U1" s="44" t="s">
+      <c r="U1" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="45"/>
     </row>
     <row r="2" spans="1:26" s="8" customFormat="1" ht="15">
       <c r="A2" s="8" t="s">
@@ -6667,13 +6667,13 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="P7" s="42" t="s">
+        <v>762</v>
+      </c>
+      <c r="Q7" s="42" t="s">
         <v>763</v>
       </c>
-      <c r="Q7" s="42" t="s">
-        <v>764</v>
-      </c>
       <c r="R7" s="42" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="32" customFormat="1">
@@ -6766,7 +6766,7 @@
         <v>22</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="E13" s="42" t="s">
         <v>77</v>
@@ -6853,7 +6853,7 @@
         <v>22</v>
       </c>
       <c r="D17" s="42" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E17" s="42" t="s">
         <v>77</v>
@@ -7182,7 +7182,7 @@
         <v>172</v>
       </c>
       <c r="F34" s="42" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="G34" s="42" t="s">
         <v>64</v>
@@ -7289,7 +7289,7 @@
         <v>172</v>
       </c>
       <c r="F39" s="42" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="G39" s="42" t="s">
         <v>64</v>
@@ -7396,7 +7396,7 @@
         <v>172</v>
       </c>
       <c r="F44" s="42" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="G44" s="42" t="s">
         <v>64</v>
@@ -7736,7 +7736,7 @@
         <v>636</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="C4" s="32" t="s">
         <v>637</v>
@@ -7769,7 +7769,7 @@
         <v>639</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C5" s="32" t="s">
         <v>640</v>
@@ -7802,7 +7802,7 @@
         <v>642</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C6" s="32" t="s">
         <v>643</v>
@@ -7835,7 +7835,7 @@
         <v>645</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>646</v>
@@ -7870,7 +7870,7 @@
       <c r="B8" s="32"/>
       <c r="C8" s="32"/>
       <c r="D8" s="32" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E8" s="32" t="s">
         <v>714</v>
@@ -7899,7 +7899,7 @@
       <c r="B9" s="32"/>
       <c r="C9" s="32"/>
       <c r="D9" s="32" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E9" s="32" t="s">
         <v>714</v>
@@ -7928,7 +7928,7 @@
       <c r="B10" s="32"/>
       <c r="C10" s="32"/>
       <c r="D10" s="32" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E10" s="32" t="s">
         <v>714</v>
@@ -7957,7 +7957,7 @@
       <c r="B11" s="32"/>
       <c r="C11" s="32"/>
       <c r="D11" s="32" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E11" s="32" t="s">
         <v>718</v>

</xml_diff>